<commit_message>
Added missing icons, all converted to 256 palette
</commit_message>
<xml_diff>
--- a/DOC/ARSO/variants.xlsx
+++ b/DOC/ARSO/variants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OGRIN\GitHub\RoomDisplay\DOC\ARSO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F829A7-9A94-4F6A-80E1-36CAD2203C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8E1175-0759-416E-9005-92607EC9CCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3AB2F3A-AC52-4CB5-9AC5-FAA5C436A82E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D3AB2F3A-AC52-4CB5-9AC5-FAA5C436A82E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="523">
   <si>
     <t>nn_icon</t>
   </si>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F223A43-61C0-4A3B-9265-5324B113745B}">
   <dimension ref="C6:I462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C209" workbookViewId="0">
-      <selection activeCell="I219" sqref="I219:I240"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I209" sqref="I209:I215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2059,7 @@
         <v>mostClear_lightFG</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" ref="G10:H73" si="1">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F10,".png")</f>
+        <f t="shared" ref="G10:G73" si="1">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F10,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/mostClear_lightFG.png</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -3457,7 +3457,7 @@
         <v>slightCloudy_FG</v>
       </c>
       <c r="G74" s="3" t="str">
-        <f t="shared" ref="G74:H137" si="3">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F74,".png")</f>
+        <f t="shared" ref="G74:G137" si="3">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F74,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/slightCloudy_FG.png</v>
       </c>
       <c r="H74" s="4" t="s">
@@ -4730,7 +4730,7 @@
         <v>_</v>
       </c>
       <c r="G138" t="str">
-        <f t="shared" ref="G138:H201" si="5">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F138,".png")</f>
+        <f t="shared" ref="G138:G201" si="5">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F138,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/_.png</v>
       </c>
       <c r="H138" s="2"/>
@@ -6133,7 +6133,7 @@
         <v>partCloudy_heavyTSGR</v>
       </c>
       <c r="G202" t="str">
-        <f t="shared" ref="G202:H265" si="7">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F202,".png")</f>
+        <f t="shared" ref="G202:G265" si="7">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F202,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/partCloudy_heavyTSGR.png</v>
       </c>
       <c r="H202" s="2" t="s">
@@ -6304,6 +6304,9 @@
       <c r="H210" s="2" t="s">
         <v>271</v>
       </c>
+      <c r="I210" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="211" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
@@ -6323,6 +6326,9 @@
       <c r="H211" s="2" t="s">
         <v>272</v>
       </c>
+      <c r="I211" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="212" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
@@ -6342,6 +6348,9 @@
       <c r="H212" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="I212" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="213" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C213" t="s">
@@ -6361,6 +6370,9 @@
       <c r="H213" s="2" t="s">
         <v>274</v>
       </c>
+      <c r="I213" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="214" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
@@ -6380,6 +6392,9 @@
       <c r="H214" s="2" t="s">
         <v>275</v>
       </c>
+      <c r="I214" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="215" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C215" t="s">
@@ -6399,6 +6414,9 @@
       <c r="H215" s="2" t="s">
         <v>276</v>
       </c>
+      <c r="I215" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="216" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C216" t="s">
@@ -6950,7 +6968,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="241" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
         <v>68</v>
       </c>
@@ -6968,8 +6986,11 @@
       <c r="H241" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="242" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I241" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="242" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C242" t="s">
         <v>68</v>
       </c>
@@ -6987,8 +7008,11 @@
       <c r="H242" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="243" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I242" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="243" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C243" t="s">
         <v>68</v>
       </c>
@@ -7006,8 +7030,11 @@
       <c r="H243" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="244" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I243" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="244" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C244" t="s">
         <v>68</v>
       </c>
@@ -7025,8 +7052,11 @@
       <c r="H244" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="245" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I244" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="245" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C245" t="s">
         <v>68</v>
       </c>
@@ -7044,8 +7074,11 @@
       <c r="H245" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="246" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I245" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="246" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C246" t="s">
         <v>68</v>
       </c>
@@ -7063,8 +7096,11 @@
       <c r="H246" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="247" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I246" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="247" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C247" t="s">
         <v>68</v>
       </c>
@@ -7082,8 +7118,11 @@
       <c r="H247" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="248" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I247" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="248" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C248" t="s">
         <v>68</v>
       </c>
@@ -7101,8 +7140,11 @@
       <c r="H248" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="249" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I248" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="249" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C249" t="s">
         <v>68</v>
       </c>
@@ -7120,8 +7162,11 @@
       <c r="H249" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="250" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I249" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="250" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C250" t="s">
         <v>68</v>
       </c>
@@ -7139,8 +7184,11 @@
       <c r="H250" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="251" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I250" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="251" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C251" t="s">
         <v>68</v>
       </c>
@@ -7158,8 +7206,11 @@
       <c r="H251" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="252" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I251" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="252" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C252" t="s">
         <v>68</v>
       </c>
@@ -7177,8 +7228,11 @@
       <c r="H252" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="253" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I252" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="253" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C253" t="s">
         <v>68</v>
       </c>
@@ -7196,8 +7250,11 @@
       <c r="H253" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="254" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I253" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="254" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C254" t="s">
         <v>68</v>
       </c>
@@ -7215,8 +7272,11 @@
       <c r="H254" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="255" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I254" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="255" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C255" t="s">
         <v>68</v>
       </c>
@@ -7234,8 +7294,11 @@
       <c r="H255" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="256" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I255" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="256" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C256" t="s">
         <v>68</v>
       </c>
@@ -7253,6 +7316,9 @@
       <c r="H256" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="I256" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="257" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C257" t="s">
@@ -7272,6 +7338,9 @@
       <c r="H257" s="2" t="s">
         <v>318</v>
       </c>
+      <c r="I257" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="258" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C258" t="s">
@@ -7291,6 +7360,9 @@
       <c r="H258" s="2" t="s">
         <v>319</v>
       </c>
+      <c r="I258" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="259" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C259" t="s">
@@ -7310,6 +7382,9 @@
       <c r="H259" s="2" t="s">
         <v>320</v>
       </c>
+      <c r="I259" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="260" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C260" t="s">
@@ -7329,6 +7404,9 @@
       <c r="H260" s="2" t="s">
         <v>321</v>
       </c>
+      <c r="I260" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="261" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C261" t="s">
@@ -7348,6 +7426,9 @@
       <c r="H261" s="2" t="s">
         <v>322</v>
       </c>
+      <c r="I261" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="262" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C262" t="s">
@@ -7367,6 +7448,9 @@
       <c r="H262" s="2" t="s">
         <v>323</v>
       </c>
+      <c r="I262" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="263" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C263" t="s">
@@ -7386,6 +7470,9 @@
       <c r="H263" s="2" t="s">
         <v>324</v>
       </c>
+      <c r="I263" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="264" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C264" t="s">
@@ -7405,6 +7492,9 @@
       <c r="H264" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="I264" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="265" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C265" t="s">
@@ -7424,6 +7514,9 @@
       <c r="H265" s="2" t="s">
         <v>326</v>
       </c>
+      <c r="I265" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="266" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C266" t="s">
@@ -7437,11 +7530,14 @@
         <v>modCloudy_modTSGR</v>
       </c>
       <c r="G266" t="str">
-        <f t="shared" ref="G266:H329" si="9">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F266,".png")</f>
+        <f t="shared" ref="G266:G329" si="9">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F266,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/modCloudy_modTSGR.png</v>
       </c>
       <c r="H266" s="2" t="s">
         <v>327</v>
+      </c>
+      <c r="I266" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="267" spans="3:9" x14ac:dyDescent="0.25">
@@ -7461,6 +7557,9 @@
       </c>
       <c r="H267" s="2" t="s">
         <v>328</v>
+      </c>
+      <c r="I267" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="268" spans="3:9" x14ac:dyDescent="0.25">
@@ -8828,7 +8927,7 @@
         <v>prevCloudy_lightTSGR</v>
       </c>
       <c r="G330" t="str">
-        <f t="shared" ref="G330:H393" si="11">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F330,".png")</f>
+        <f t="shared" ref="G330:G393" si="11">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F330,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/prevCloudy_lightTSGR.png</v>
       </c>
       <c r="H330" s="2" t="s">
@@ -10225,7 +10324,7 @@
         <v>overcast_TSGR</v>
       </c>
       <c r="G394" t="str">
-        <f t="shared" ref="G394:H457" si="13">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F394,".png")</f>
+        <f t="shared" ref="G394:G457" si="13">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F394,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/overcast_TSGR.png</v>
       </c>
       <c r="H394" s="2" t="s">
@@ -10330,6 +10429,9 @@
       <c r="H399" s="2" t="s">
         <v>457</v>
       </c>
+      <c r="I399" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="400" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C400" t="s">
@@ -10349,8 +10451,11 @@
       <c r="H400" s="2" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="401" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I400" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="401" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C401" t="s">
         <v>1</v>
       </c>
@@ -10368,8 +10473,11 @@
       <c r="H401" s="2" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="402" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I401" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="402" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C402" t="s">
         <v>1</v>
       </c>
@@ -10387,8 +10495,11 @@
       <c r="H402" s="2" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="403" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I402" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="403" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C403" t="s">
         <v>1</v>
       </c>
@@ -10406,8 +10517,11 @@
       <c r="H403" s="2" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="404" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I403" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="404" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C404" t="s">
         <v>1</v>
       </c>
@@ -10425,8 +10539,11 @@
       <c r="H404" s="2" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="405" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I404" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="405" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C405" t="s">
         <v>1</v>
       </c>
@@ -10444,8 +10561,11 @@
       <c r="H405" s="2" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="406" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I405" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="406" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C406" t="s">
         <v>1</v>
       </c>
@@ -10463,8 +10583,11 @@
       <c r="H406" s="2" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="407" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I406" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="407" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C407" t="s">
         <v>1</v>
       </c>
@@ -10482,8 +10605,11 @@
       <c r="H407" s="2" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="408" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I407" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="408" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C408" t="s">
         <v>1</v>
       </c>
@@ -10501,8 +10627,11 @@
       <c r="H408" s="2" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="409" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I408" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="409" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C409" t="s">
         <v>1</v>
       </c>
@@ -10520,8 +10649,11 @@
       <c r="H409" s="2" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="410" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I409" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="410" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C410" t="s">
         <v>1</v>
       </c>
@@ -10539,8 +10671,11 @@
       <c r="H410" s="2" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="411" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I410" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="411" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C411" t="s">
         <v>1</v>
       </c>
@@ -10558,8 +10693,11 @@
       <c r="H411" s="2" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="412" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I411" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="412" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C412" t="s">
         <v>1</v>
       </c>
@@ -10577,8 +10715,11 @@
       <c r="H412" s="2" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="413" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I412" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="413" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C413" t="s">
         <v>1</v>
       </c>
@@ -10596,8 +10737,11 @@
       <c r="H413" s="2" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="414" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I413" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="414" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C414" t="s">
         <v>1</v>
       </c>
@@ -10615,8 +10759,11 @@
       <c r="H414" s="2" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="415" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I414" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="415" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C415" t="s">
         <v>1</v>
       </c>
@@ -10634,8 +10781,11 @@
       <c r="H415" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="416" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I415" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="416" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C416" t="s">
         <v>1</v>
       </c>
@@ -10653,8 +10803,11 @@
       <c r="H416" s="2" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="417" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I416" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="417" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C417" t="s">
         <v>1</v>
       </c>
@@ -10672,8 +10825,11 @@
       <c r="H417" s="2" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="418" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I417" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="418" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C418" t="s">
         <v>1</v>
       </c>
@@ -10691,8 +10847,11 @@
       <c r="H418" s="2" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="419" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I418" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="419" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C419" t="s">
         <v>1</v>
       </c>
@@ -10710,8 +10869,11 @@
       <c r="H419" s="2" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="420" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I419" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="420" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C420" t="s">
         <v>1</v>
       </c>
@@ -10729,8 +10891,11 @@
       <c r="H420" s="2" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="421" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I420" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="421" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C421" t="s">
         <v>1</v>
       </c>
@@ -10748,8 +10913,11 @@
       <c r="H421" s="2" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="422" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I421" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="422" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C422" t="s">
         <v>1</v>
       </c>
@@ -10767,8 +10935,11 @@
       <c r="H422" s="2" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="423" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I422" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="423" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C423" t="s">
         <v>1</v>
       </c>
@@ -10786,8 +10957,11 @@
       <c r="H423" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="424" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I423" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="424" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C424" t="s">
         <v>1</v>
       </c>
@@ -10805,8 +10979,11 @@
       <c r="H424" s="2" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="425" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I424" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="425" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C425" t="s">
         <v>1</v>
       </c>
@@ -10824,8 +11001,11 @@
       <c r="H425" s="2" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="426" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I425" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="426" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C426" t="s">
         <v>1</v>
       </c>
@@ -10843,8 +11023,11 @@
       <c r="H426" s="2" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="427" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I426" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="427" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C427" t="s">
         <v>1</v>
       </c>
@@ -10862,8 +11045,11 @@
       <c r="H427" s="2" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="428" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I427" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="428" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C428" t="s">
         <v>1</v>
       </c>
@@ -10881,8 +11067,11 @@
       <c r="H428" s="2" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="429" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I428" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="429" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C429" t="s">
         <v>1</v>
       </c>
@@ -10900,8 +11089,11 @@
       <c r="H429" s="2" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="430" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I429" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="430" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C430" t="s">
         <v>1</v>
       </c>
@@ -10919,8 +11111,11 @@
       <c r="H430" s="2" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="431" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I430" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="431" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C431" t="s">
         <v>1</v>
       </c>
@@ -10938,8 +11133,11 @@
       <c r="H431" s="2" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="432" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I431" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="432" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C432" t="s">
         <v>1</v>
       </c>
@@ -10957,8 +11155,11 @@
       <c r="H432" s="2" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="433" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I432" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="433" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C433" t="s">
         <v>1</v>
       </c>
@@ -10976,8 +11177,11 @@
       <c r="H433" s="2" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="434" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I433" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="434" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C434" t="s">
         <v>1</v>
       </c>
@@ -10995,8 +11199,11 @@
       <c r="H434" s="2" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="435" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I434" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="435" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C435" t="s">
         <v>1</v>
       </c>
@@ -11014,8 +11221,11 @@
       <c r="H435" s="2" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="436" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I435" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="436" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C436" t="s">
         <v>1</v>
       </c>
@@ -11033,8 +11243,11 @@
       <c r="H436" s="2" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="437" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I436" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="437" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C437" t="s">
         <v>1</v>
       </c>
@@ -11052,8 +11265,11 @@
       <c r="H437" s="2" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="438" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I437" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="438" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C438" t="s">
         <v>1</v>
       </c>
@@ -11071,8 +11287,11 @@
       <c r="H438" s="2" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="439" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I438" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="439" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C439" t="s">
         <v>1</v>
       </c>
@@ -11090,8 +11309,11 @@
       <c r="H439" s="2" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="440" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I439" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="440" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C440" t="s">
         <v>1</v>
       </c>
@@ -11109,8 +11331,11 @@
       <c r="H440" s="2" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="441" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I440" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="441" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C441" t="s">
         <v>1</v>
       </c>
@@ -11128,8 +11353,11 @@
       <c r="H441" s="2" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="442" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I441" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="442" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C442" t="s">
         <v>1</v>
       </c>
@@ -11147,8 +11375,11 @@
       <c r="H442" s="2" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="443" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I442" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="443" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C443" t="s">
         <v>1</v>
       </c>
@@ -11166,8 +11397,11 @@
       <c r="H443" s="2" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="444" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I443" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="444" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C444" t="s">
         <v>1</v>
       </c>
@@ -11185,8 +11419,11 @@
       <c r="H444" s="2" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="445" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I444" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="445" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C445" t="s">
         <v>1</v>
       </c>
@@ -11204,8 +11441,11 @@
       <c r="H445" s="2" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="446" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I445" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="446" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C446" t="s">
         <v>1</v>
       </c>
@@ -11223,8 +11463,11 @@
       <c r="H446" s="2" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="447" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I446" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="447" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C447" t="s">
         <v>1</v>
       </c>
@@ -11242,8 +11485,11 @@
       <c r="H447" s="2" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="448" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I447" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="448" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C448" t="s">
         <v>1</v>
       </c>
@@ -11261,8 +11507,11 @@
       <c r="H448" s="2" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="449" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I448" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="449" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C449" t="s">
         <v>1</v>
       </c>
@@ -11280,8 +11529,11 @@
       <c r="H449" s="2" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="450" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I449" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="450" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C450" t="s">
         <v>1</v>
       </c>
@@ -11299,8 +11551,11 @@
       <c r="H450" s="2" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="451" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I450" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="451" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C451" t="s">
         <v>1</v>
       </c>
@@ -11318,8 +11573,11 @@
       <c r="H451" s="2" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="452" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I451" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="452" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C452" t="s">
         <v>1</v>
       </c>
@@ -11337,8 +11595,11 @@
       <c r="H452" s="2" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="453" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I452" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="453" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C453" t="s">
         <v>1</v>
       </c>
@@ -11356,8 +11617,11 @@
       <c r="H453" s="2" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="454" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I453" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="454" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C454" t="s">
         <v>1</v>
       </c>
@@ -11375,8 +11639,11 @@
       <c r="H454" s="2" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="455" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I454" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="455" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C455" t="s">
         <v>1</v>
       </c>
@@ -11394,8 +11661,11 @@
       <c r="H455" s="2" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="456" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I455" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="456" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C456" t="s">
         <v>1</v>
       </c>
@@ -11413,8 +11683,11 @@
       <c r="H456" s="2" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="457" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I456" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="457" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C457" t="s">
         <v>1</v>
       </c>
@@ -11432,8 +11705,11 @@
       <c r="H457" s="2" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="458" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I457" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="458" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C458" t="s">
         <v>1</v>
       </c>
@@ -11445,14 +11721,17 @@
         <v>FG_heavyTSSN</v>
       </c>
       <c r="G458" t="str">
-        <f t="shared" ref="G458:H462" si="15">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F458,".png")</f>
+        <f t="shared" ref="G458:G462" si="15">_xlfn.CONCAT("https://meteo.arso.gov.si/uploads/meteo/style/img/weather/",F458,".png")</f>
         <v>https://meteo.arso.gov.si/uploads/meteo/style/img/weather/FG_heavyTSSN.png</v>
       </c>
       <c r="H458" s="2" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="459" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I458" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="459" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C459" t="s">
         <v>1</v>
       </c>
@@ -11470,8 +11749,11 @@
       <c r="H459" s="2" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="460" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I459" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="460" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C460" t="s">
         <v>1</v>
       </c>
@@ -11489,8 +11771,11 @@
       <c r="H460" s="2" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="461" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I460" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="461" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C461" t="s">
         <v>1</v>
       </c>
@@ -11508,8 +11793,11 @@
       <c r="H461" s="2" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="462" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I461" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="462" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C462" t="s">
         <v>1</v>
       </c>
@@ -11526,6 +11814,9 @@
       </c>
       <c r="H462" s="2" t="s">
         <v>520</v>
+      </c>
+      <c r="I462" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>